<commit_message>
Changed end year to peak year
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -49,7 +49,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">(Required) The approximate year the aesthetic started.</t>
+          <t xml:space="preserve">The year of the first known example of the aesthetic.</t>
         </r>
       </text>
     </comment>
@@ -288,6 +288,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The way in which the target aesthetic is related to the subject aesthetic.</t>
         </r>
@@ -306,7 +307,7 @@
     <t xml:space="preserve">start_year</t>
   </si>
   <si>
-    <t xml:space="preserve">end_year</t>
+    <t xml:space="preserve">peak_year</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
@@ -358,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -386,11 +387,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -441,12 +437,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -542,14 +542,14 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.02"/>
@@ -562,7 +562,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -585,10 +585,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="2"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="2"/>
+      <c r="D52" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -613,7 +613,7 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.51"/>
@@ -648,24 +648,24 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -690,7 +690,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.1"/>
@@ -713,32 +713,32 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="4"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="4"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="4"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="4"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="4"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="4"/>
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>